<commit_message>
adds first emissions to database
</commit_message>
<xml_diff>
--- a/static/data/Abschnitt I Fliegen(1).xlsx
+++ b/static/data/Abschnitt I Fliegen(1).xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon Schneider\PycharmProjects\co2besser\static\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="345" windowWidth="19875" windowHeight="7725"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Emission gesamt" sheetId="1" r:id="rId1"/>
     <sheet name="Kurz- Mittel- und Langstrecken" sheetId="2" r:id="rId2"/>
     <sheet name="Flugverhalten" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -226,13 +231,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="#,##0_ ;\-#,##0\ "/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -291,36 +296,36 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -338,7 +343,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -364,14 +369,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -409,9 +417,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -446,7 +454,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -481,7 +489,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -657,40 +665,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="62.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="57.42578125" customWidth="1"/>
+    <col min="1" max="1" width="62.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="57.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:4" s="25" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="25" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>50</v>
       </c>
@@ -698,13 +706,13 @@
       <c r="C4" s="35"/>
       <c r="D4" s="35"/>
     </row>
-    <row r="5" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26"/>
       <c r="B5" s="26"/>
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
     </row>
-    <row r="6" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>51</v>
       </c>
@@ -712,7 +720,7 @@
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
     </row>
-    <row r="7" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>56</v>
       </c>
@@ -721,7 +729,7 @@
         <v>8500000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>57</v>
       </c>
@@ -730,7 +738,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>58</v>
       </c>
@@ -740,7 +748,7 @@
         <v>10625000000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>59</v>
       </c>
@@ -749,7 +757,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>60</v>
       </c>
@@ -759,7 +767,7 @@
         <v>252976190476.19046</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
         <v>63</v>
       </c>
@@ -768,7 +776,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="31" t="s">
         <v>64</v>
       </c>
@@ -778,7 +786,7 @@
         <v>151785714285.71426</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>61</v>
       </c>
@@ -787,7 +795,7 @@
         <v>82500000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
         <v>62</v>
       </c>
@@ -797,17 +805,17 @@
         <v>1839.8268398268397</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="31"/>
       <c r="C16" s="8"/>
       <c r="D16" s="30"/>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26"/>
       <c r="B17" s="10"/>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>52</v>
       </c>
@@ -821,12 +829,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>5</v>
       </c>
@@ -842,7 +850,7 @@
         <v>107.64</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>6</v>
       </c>
@@ -858,7 +866,7 @@
         <v>43.792000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>7</v>
       </c>
@@ -874,7 +882,7 @@
         <v>51.887999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>0</v>
       </c>
@@ -890,12 +898,12 @@
         <v>203.32000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="10"/>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>53</v>
       </c>
@@ -906,12 +914,12 @@
         <v>345.64400000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="12"/>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>67</v>
       </c>
@@ -919,14 +927,14 @@
       <c r="C27" s="8"/>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -937,7 +945,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -948,7 +956,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -960,7 +968,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -971,7 +979,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -982,7 +990,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34"/>
       <c r="B34" s="10">
         <f>B32*B33/1000</f>
@@ -992,7 +1000,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -1001,7 +1009,7 @@
       </c>
       <c r="C35"/>
     </row>
-    <row r="36" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>23</v>
       </c>
@@ -1013,7 +1021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37"/>
       <c r="B37" s="10">
         <v>8400000</v>
@@ -1023,7 +1031,7 @@
       </c>
       <c r="D37" s="19"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>54</v>
       </c>
@@ -1033,12 +1041,12 @@
         <v>35.736747529200358</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="8"/>
       <c r="B39" s="11"/>
       <c r="C39" s="8"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>55</v>
       </c>
@@ -1047,7 +1055,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
         <v>24</v>
       </c>
@@ -1058,19 +1066,19 @@
         <v>594.70074752920038</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="21"/>
       <c r="C46" s="5"/>
@@ -1092,21 +1100,21 @@
       <selection activeCell="I4" sqref="I4:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -1124,7 +1132,7 @@
       <c r="O2" s="3"/>
       <c r="P2"/>
     </row>
-    <row r="3" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>27</v>
       </c>
@@ -1157,7 +1165,7 @@
       </c>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>26</v>
       </c>
@@ -1195,7 +1203,7 @@
       </c>
       <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
@@ -1232,7 +1240,7 @@
         <v>1041.0119999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
@@ -1269,7 +1277,7 @@
         <v>657.84960000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="13"/>
@@ -1281,7 +1289,7 @@
       <c r="I7" s="7"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
         <v>36</v>
       </c>
@@ -1295,27 +1303,27 @@
       <c r="I8" s="36"/>
       <c r="J8" s="36"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I9" s="3"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I10" s="3"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I11" s="3"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I12" s="3"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I13" s="3"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1325,34 +1333,34 @@
       <c r="I14" s="7"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I16" s="3"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I17" s="3"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I18" s="3"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I19" s="3"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I20" s="3"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I21" s="3"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1362,26 +1370,26 @@
       <c r="I22" s="7"/>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I24" s="3"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I25" s="3"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I26" s="3"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.3">
       <c r="I27" s="3"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -1404,24 +1412,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1453,10 +1461,10 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1485,8 +1493,16 @@
         <f>D4*G4/1000</f>
         <v>2914.8335999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4" s="19">
+        <f t="shared" ref="I4:I7" si="0">H4*0.08</f>
+        <v>233.186688</v>
+      </c>
+      <c r="J4" s="34">
+        <f t="shared" ref="J4:J7" si="1">H4+I4</f>
+        <v>3148.0202879999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>40</v>
       </c>
@@ -1501,19 +1517,27 @@
         <v>7.46</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" ref="F5:F7" si="0">E5*2.52*10</f>
+        <f t="shared" ref="F5:F7" si="2">E5*2.52*10</f>
         <v>187.99199999999999</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" ref="G5:G7" si="1">F5*2.7</f>
+        <f t="shared" ref="G5:G7" si="3">F5*2.7</f>
         <v>507.57839999999999</v>
       </c>
       <c r="H5" s="10">
         <f>D5*G5/1000</f>
         <v>609.09407999999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="19">
+        <f t="shared" si="0"/>
+        <v>48.727526399999995</v>
+      </c>
+      <c r="J5" s="34">
+        <f t="shared" si="1"/>
+        <v>657.82160639999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>41</v>
       </c>
@@ -1528,19 +1552,27 @@
         <v>7.46</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>187.99199999999999</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>507.57839999999999</v>
       </c>
       <c r="H6" s="10">
         <f>D6*G6/1000</f>
         <v>609.09407999999996</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I6" s="19">
+        <f t="shared" si="0"/>
+        <v>48.727526399999995</v>
+      </c>
+      <c r="J6" s="34">
+        <f t="shared" si="1"/>
+        <v>657.82160639999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
         <v>42</v>
       </c>
@@ -1555,19 +1587,27 @@
         <v>7.46</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>187.99199999999999</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>507.57839999999999</v>
       </c>
       <c r="H7" s="10">
         <f>D7*G7/1000</f>
         <v>609.09407999999996</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I7" s="19">
+        <f t="shared" si="0"/>
+        <v>48.727526399999995</v>
+      </c>
+      <c r="J7" s="34">
+        <f t="shared" si="1"/>
+        <v>657.82160639999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
         <v>0</v>
       </c>
@@ -1589,12 +1629,12 @@
         <v>5121.4851071999992</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E9" s="3"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -1612,11 +1652,11 @@
         <v>4.7300000000000004</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" ref="F10:F12" si="2">E10*2.52*10</f>
+        <f t="shared" ref="F10:F12" si="4">E10*2.52*10</f>
         <v>119.19600000000001</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" ref="G10:G12" si="3">F10*2.7</f>
+        <f t="shared" ref="G10:G12" si="5">F10*2.7</f>
         <v>321.82920000000007</v>
       </c>
       <c r="H10" s="10">
@@ -1626,7 +1666,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
         <v>40</v>
       </c>
@@ -1641,11 +1681,11 @@
         <v>7.46</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>187.99199999999999</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>507.57839999999999</v>
       </c>
       <c r="H11" s="10">
@@ -1655,7 +1695,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>41</v>
       </c>
@@ -1670,11 +1710,11 @@
         <v>7.46</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>187.99199999999999</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>507.57839999999999</v>
       </c>
       <c r="H12" s="10">
@@ -1684,7 +1724,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="s">
         <v>0</v>
       </c>
@@ -1706,12 +1746,12 @@
         <v>2358.3698208000001</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E14" s="3"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1733,7 +1773,7 @@
         <v>119.19600000000001</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" ref="G15" si="4">F15*2.7</f>
+        <f t="shared" ref="G15" si="6">F15*2.7</f>
         <v>321.82920000000007</v>
       </c>
       <c r="H15" s="10">
@@ -1743,7 +1783,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="9" t="s">
         <v>0</v>
       </c>
@@ -1765,7 +1805,7 @@
         <v>1042.7266080000002</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D17" s="10"/>
       <c r="E17" s="22"/>
       <c r="F17" s="2"/>
@@ -1774,7 +1814,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -1796,7 +1836,7 @@
         <v>119.19600000000001</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" ref="G18" si="5">F18*2.7</f>
+        <f t="shared" ref="G18" si="7">F18*2.7</f>
         <v>321.82920000000007</v>
       </c>
       <c r="H18" s="10">
@@ -1806,7 +1846,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B19" s="9" t="s">
         <v>0</v>
       </c>
@@ -1828,67 +1868,67 @@
         <v>104.27266080000004</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D20" s="10"/>
       <c r="E20" s="22"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="10"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D21" s="10"/>
       <c r="E21" s="22"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E22" s="3"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E23" s="3"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E24" s="3"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E25" s="3"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E26" s="3"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="7"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E29" s="3"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E30" s="3"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E31" s="3"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E32" s="3"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>

</xml_diff>